<commit_message>
Fix Excel workbook: use formulas for progress, export VBA as .bas
The hand-crafted OLE binary for VBA injection was causing Excel to
error on open. Replaced with a reliable approach:

- Dashboard now uses SUMPRODUCT/COUNTA formulas that auto-update as
  users fill in responses — no macros needed for progress tracking
- VBA code exported as GreenStarMacros.bas and ThisWorkbook.cls for
  optional manual import (Developer > VBA Editor > Import File)
- Removed the custom OLE compound document builder (unreliable)
- Removed the broken .xlsm file
- Updated instructions on Dashboard to reflect formula-based progress
  and optional VBA import steps

The .xlsx works immediately out of the box. VBA is optional for
advanced features (conditional visibility, search, review, dark mode).

https://claude.ai/code/session_015zL8AEuvfUGA59cjgfEpnA
</commit_message>
<xml_diff>
--- a/Green_Star_Buildings_v1.1_Interactive.xlsx
+++ b/Green_Star_Buildings_v1.1_Interactive.xlsx
@@ -780,14 +780,17 @@
       </c>
       <c r="B2" s="3" t="inlineStr"/>
       <c r="C2" s="3" t="inlineStr"/>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>375</v>
-      </c>
-      <c r="F2" s="4" t="n">
-        <v>0</v>
+      <c r="D2" s="3">
+        <f>SUM(D5:D48)</f>
+        <v/>
+      </c>
+      <c r="E2" s="3">
+        <f>SUM(E5:E48)</f>
+        <v/>
+      </c>
+      <c r="F2" s="4">
+        <f>IF(E2&gt;0,D2/E2,0)</f>
+        <v/>
       </c>
     </row>
     <row r="3" ht="10" customHeight="1"/>
@@ -835,14 +838,17 @@
         </is>
       </c>
       <c r="C5" s="8" t="n"/>
-      <c r="D5" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="F5" s="10" t="n">
-        <v>0</v>
+      <c r="D5" s="9">
+        <f>SUMPRODUCT(('Industry Development'!E6:E22&lt;&gt;"")*('Industry Development'!G6:G22&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E5" s="9">
+        <f>COUNTA('Industry Development'!E6:E22)</f>
+        <v/>
+      </c>
+      <c r="F5" s="10">
+        <f>IF(E5&gt;0,D5/E5,0)</f>
+        <v/>
       </c>
     </row>
     <row r="6" ht="22" customHeight="1">
@@ -857,14 +863,17 @@
         </is>
       </c>
       <c r="C6" s="8" t="n"/>
-      <c r="D6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>0</v>
+      <c r="D6" s="9">
+        <f>SUMPRODUCT(('Responsible Construction'!E6:E35&lt;&gt;"")*('Responsible Construction'!G6:G35&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E6" s="9">
+        <f>COUNTA('Responsible Construction'!E6:E35)</f>
+        <v/>
+      </c>
+      <c r="F6" s="10">
+        <f>IF(E6&gt;0,D6/E6,0)</f>
+        <v/>
       </c>
     </row>
     <row r="7" ht="22" customHeight="1">
@@ -879,14 +888,17 @@
         </is>
       </c>
       <c r="C7" s="8" t="n"/>
-      <c r="D7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9" t="n">
-        <v>35</v>
-      </c>
-      <c r="F7" s="10" t="n">
-        <v>0</v>
+      <c r="D7" s="9">
+        <f>SUMPRODUCT(('Verification and Handover'!E6:E46&lt;&gt;"")*('Verification and Handover'!G6:G46&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E7" s="9">
+        <f>COUNTA('Verification and Handover'!E6:E46)</f>
+        <v/>
+      </c>
+      <c r="F7" s="10">
+        <f>IF(E7&gt;0,D7/E7,0)</f>
+        <v/>
       </c>
     </row>
     <row r="8" ht="22" customHeight="1">
@@ -901,14 +913,17 @@
         </is>
       </c>
       <c r="C8" s="8" t="n"/>
-      <c r="D8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="F8" s="10" t="n">
-        <v>0</v>
+      <c r="D8" s="9">
+        <f>SUMPRODUCT(('Responsible Resource Mgmt'!E6:E23&lt;&gt;"")*('Responsible Resource Mgmt'!G6:G23&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E8" s="9">
+        <f>COUNTA('Responsible Resource Mgmt'!E6:E23)</f>
+        <v/>
+      </c>
+      <c r="F8" s="10">
+        <f>IF(E8&gt;0,D8/E8,0)</f>
+        <v/>
       </c>
     </row>
     <row r="9" ht="22" customHeight="1">
@@ -923,14 +938,17 @@
         </is>
       </c>
       <c r="C9" s="8" t="n"/>
-      <c r="D9" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>0</v>
+      <c r="D9" s="9">
+        <f>SUMPRODUCT(('Responsible Procurement'!E6:E22&lt;&gt;"")*('Responsible Procurement'!G6:G22&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E9" s="9">
+        <f>COUNTA('Responsible Procurement'!E6:E22)</f>
+        <v/>
+      </c>
+      <c r="F9" s="10">
+        <f>IF(E9&gt;0,D9/E9,0)</f>
+        <v/>
       </c>
     </row>
     <row r="10" ht="22" customHeight="1">
@@ -945,14 +963,17 @@
         </is>
       </c>
       <c r="C10" s="8" t="n"/>
-      <c r="D10" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>0</v>
+      <c r="D10" s="9">
+        <f>SUMPRODUCT(('Responsible Structure'!E6:E15&lt;&gt;"")*('Responsible Structure'!G6:G15&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E10" s="9">
+        <f>COUNTA('Responsible Structure'!E6:E15)</f>
+        <v/>
+      </c>
+      <c r="F10" s="10">
+        <f>IF(E10&gt;0,D10/E10,0)</f>
+        <v/>
       </c>
     </row>
     <row r="11" ht="22" customHeight="1">
@@ -967,14 +988,17 @@
         </is>
       </c>
       <c r="C11" s="8" t="n"/>
-      <c r="D11" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>0</v>
+      <c r="D11" s="9">
+        <f>SUMPRODUCT(('Responsible Envelope'!E6:E12&lt;&gt;"")*('Responsible Envelope'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E11" s="9">
+        <f>COUNTA('Responsible Envelope'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F11" s="10">
+        <f>IF(E11&gt;0,D11/E11,0)</f>
+        <v/>
       </c>
     </row>
     <row r="12" ht="22" customHeight="1">
@@ -989,14 +1013,17 @@
         </is>
       </c>
       <c r="C12" s="8" t="n"/>
-      <c r="D12" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F12" s="10" t="n">
-        <v>0</v>
+      <c r="D12" s="9">
+        <f>SUMPRODUCT(('Responsible Systems'!E6:E12&lt;&gt;"")*('Responsible Systems'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E12" s="9">
+        <f>COUNTA('Responsible Systems'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F12" s="10">
+        <f>IF(E12&gt;0,D12/E12,0)</f>
+        <v/>
       </c>
     </row>
     <row r="13" ht="22" customHeight="1">
@@ -1011,14 +1038,17 @@
         </is>
       </c>
       <c r="C13" s="8" t="n"/>
-      <c r="D13" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F13" s="10" t="n">
-        <v>0</v>
+      <c r="D13" s="9">
+        <f>SUMPRODUCT(('Responsible Finishes'!E6:E12&lt;&gt;"")*('Responsible Finishes'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E13" s="9">
+        <f>COUNTA('Responsible Finishes'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F13" s="10">
+        <f>IF(E13&gt;0,D13/E13,0)</f>
+        <v/>
       </c>
     </row>
     <row r="14" ht="22" customHeight="1">
@@ -1033,14 +1063,17 @@
         </is>
       </c>
       <c r="C14" s="8" t="n"/>
-      <c r="D14" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F14" s="10" t="n">
-        <v>0</v>
+      <c r="D14" s="9">
+        <f>SUMPRODUCT(('Impacts Disclosure'!E6:E16&lt;&gt;"")*('Impacts Disclosure'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E14" s="9">
+        <f>COUNTA('Impacts Disclosure'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F14" s="10">
+        <f>IF(E14&gt;0,D14/E14,0)</f>
+        <v/>
       </c>
     </row>
     <row r="15" ht="22" customHeight="1">
@@ -1055,14 +1088,17 @@
         </is>
       </c>
       <c r="C15" s="11" t="n"/>
-      <c r="D15" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="F15" s="10" t="n">
-        <v>0</v>
+      <c r="D15" s="9">
+        <f>SUMPRODUCT(('Clean Air'!E6:E22&lt;&gt;"")*('Clean Air'!G6:G22&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E15" s="9">
+        <f>COUNTA('Clean Air'!E6:E22)</f>
+        <v/>
+      </c>
+      <c r="F15" s="10">
+        <f>IF(E15&gt;0,D15/E15,0)</f>
+        <v/>
       </c>
     </row>
     <row r="16" ht="22" customHeight="1">
@@ -1077,14 +1113,17 @@
         </is>
       </c>
       <c r="C16" s="11" t="n"/>
-      <c r="D16" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9" t="n">
-        <v>12</v>
-      </c>
-      <c r="F16" s="10" t="n">
-        <v>0</v>
+      <c r="D16" s="9">
+        <f>SUMPRODUCT(('Light Quality'!E6:E23&lt;&gt;"")*('Light Quality'!G6:G23&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E16" s="9">
+        <f>COUNTA('Light Quality'!E6:E23)</f>
+        <v/>
+      </c>
+      <c r="F16" s="10">
+        <f>IF(E16&gt;0,D16/E16,0)</f>
+        <v/>
       </c>
     </row>
     <row r="17" ht="22" customHeight="1">
@@ -1099,14 +1138,17 @@
         </is>
       </c>
       <c r="C17" s="11" t="n"/>
-      <c r="D17" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="F17" s="10" t="n">
-        <v>0</v>
+      <c r="D17" s="9">
+        <f>SUMPRODUCT(('Acoustic Comfort'!E6:E25&lt;&gt;"")*('Acoustic Comfort'!G6:G25&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E17" s="9">
+        <f>COUNTA('Acoustic Comfort'!E6:E25)</f>
+        <v/>
+      </c>
+      <c r="F17" s="10">
+        <f>IF(E17&gt;0,D17/E17,0)</f>
+        <v/>
       </c>
     </row>
     <row r="18" ht="22" customHeight="1">
@@ -1121,14 +1163,17 @@
         </is>
       </c>
       <c r="C18" s="11" t="n"/>
-      <c r="D18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="F18" s="10" t="n">
-        <v>0</v>
+      <c r="D18" s="9">
+        <f>SUMPRODUCT(('Exposure to Toxins'!E6:E18&lt;&gt;"")*('Exposure to Toxins'!G6:G18&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E18" s="9">
+        <f>COUNTA('Exposure to Toxins'!E6:E18)</f>
+        <v/>
+      </c>
+      <c r="F18" s="10">
+        <f>IF(E18&gt;0,D18/E18,0)</f>
+        <v/>
       </c>
     </row>
     <row r="19" ht="22" customHeight="1">
@@ -1143,14 +1188,17 @@
         </is>
       </c>
       <c r="C19" s="11" t="n"/>
-      <c r="D19" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F19" s="10" t="n">
-        <v>0</v>
+      <c r="D19" s="9">
+        <f>SUMPRODUCT(('Amenity and Comfort'!E6:E16&lt;&gt;"")*('Amenity and Comfort'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E19" s="9">
+        <f>COUNTA('Amenity and Comfort'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F19" s="10">
+        <f>IF(E19&gt;0,D19/E19,0)</f>
+        <v/>
       </c>
     </row>
     <row r="20" ht="22" customHeight="1">
@@ -1165,14 +1213,17 @@
         </is>
       </c>
       <c r="C20" s="11" t="n"/>
-      <c r="D20" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F20" s="10" t="n">
-        <v>0</v>
+      <c r="D20" s="9">
+        <f>SUMPRODUCT(('Connection to Nature'!E6:E16&lt;&gt;"")*('Connection to Nature'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E20" s="9">
+        <f>COUNTA('Connection to Nature'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F20" s="10">
+        <f>IF(E20&gt;0,D20/E20,0)</f>
+        <v/>
       </c>
     </row>
     <row r="21" ht="22" customHeight="1">
@@ -1187,14 +1238,17 @@
         </is>
       </c>
       <c r="C21" s="12" t="n"/>
-      <c r="D21" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F21" s="10" t="n">
-        <v>0</v>
+      <c r="D21" s="9">
+        <f>SUMPRODUCT(('Climate Resilience'!E6:E16&lt;&gt;"")*('Climate Resilience'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E21" s="9">
+        <f>COUNTA('Climate Resilience'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F21" s="10">
+        <f>IF(E21&gt;0,D21/E21,0)</f>
+        <v/>
       </c>
     </row>
     <row r="22" ht="22" customHeight="1">
@@ -1209,14 +1263,17 @@
         </is>
       </c>
       <c r="C22" s="12" t="n"/>
-      <c r="D22" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F22" s="10" t="n">
-        <v>0</v>
+      <c r="D22" s="9">
+        <f>SUMPRODUCT(('Operations Resilience'!E6:E13&lt;&gt;"")*('Operations Resilience'!G6:G13&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E22" s="9">
+        <f>COUNTA('Operations Resilience'!E6:E13)</f>
+        <v/>
+      </c>
+      <c r="F22" s="10">
+        <f>IF(E22&gt;0,D22/E22,0)</f>
+        <v/>
       </c>
     </row>
     <row r="23" ht="22" customHeight="1">
@@ -1231,14 +1288,17 @@
         </is>
       </c>
       <c r="C23" s="12" t="n"/>
-      <c r="D23" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F23" s="10" t="n">
-        <v>0</v>
+      <c r="D23" s="9">
+        <f>SUMPRODUCT(('Community Resilience'!E6:E9&lt;&gt;"")*('Community Resilience'!G6:G9&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E23" s="9">
+        <f>COUNTA('Community Resilience'!E6:E9)</f>
+        <v/>
+      </c>
+      <c r="F23" s="10">
+        <f>IF(E23&gt;0,D23/E23,0)</f>
+        <v/>
       </c>
     </row>
     <row r="24" ht="22" customHeight="1">
@@ -1253,14 +1313,17 @@
         </is>
       </c>
       <c r="C24" s="12" t="n"/>
-      <c r="D24" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F24" s="10" t="n">
-        <v>0</v>
+      <c r="D24" s="9">
+        <f>SUMPRODUCT(('Heat Resilience'!E6:E12&lt;&gt;"")*('Heat Resilience'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E24" s="9">
+        <f>COUNTA('Heat Resilience'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F24" s="10">
+        <f>IF(E24&gt;0,D24/E24,0)</f>
+        <v/>
       </c>
     </row>
     <row r="25" ht="22" customHeight="1">
@@ -1275,14 +1338,17 @@
         </is>
       </c>
       <c r="C25" s="12" t="n"/>
-      <c r="D25" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F25" s="10" t="n">
-        <v>0</v>
+      <c r="D25" s="9">
+        <f>SUMPRODUCT(('Grid Resilience'!E6:E15&lt;&gt;"")*('Grid Resilience'!G6:G15&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E25" s="9">
+        <f>COUNTA('Grid Resilience'!E6:E15)</f>
+        <v/>
+      </c>
+      <c r="F25" s="10">
+        <f>IF(E25&gt;0,D25/E25,0)</f>
+        <v/>
       </c>
     </row>
     <row r="26" ht="22" customHeight="1">
@@ -1297,14 +1363,17 @@
         </is>
       </c>
       <c r="C26" s="13" t="n"/>
-      <c r="D26" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="F26" s="10" t="n">
-        <v>0</v>
+      <c r="D26" s="9">
+        <f>SUMPRODUCT(('Energy Source'!E6:E21&lt;&gt;"")*('Energy Source'!G6:G21&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E26" s="9">
+        <f>COUNTA('Energy Source'!E6:E21)</f>
+        <v/>
+      </c>
+      <c r="F26" s="10">
+        <f>IF(E26&gt;0,D26/E26,0)</f>
+        <v/>
       </c>
     </row>
     <row r="27" ht="22" customHeight="1">
@@ -1319,14 +1388,17 @@
         </is>
       </c>
       <c r="C27" s="13" t="n"/>
-      <c r="D27" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="F27" s="10" t="n">
-        <v>0</v>
+      <c r="D27" s="9">
+        <f>SUMPRODUCT(('Energy Use'!E6:E20&lt;&gt;"")*('Energy Use'!G6:G20&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E27" s="9">
+        <f>COUNTA('Energy Use'!E6:E20)</f>
+        <v/>
+      </c>
+      <c r="F27" s="10">
+        <f>IF(E27&gt;0,D27/E27,0)</f>
+        <v/>
       </c>
     </row>
     <row r="28" ht="22" customHeight="1">
@@ -1341,14 +1413,17 @@
         </is>
       </c>
       <c r="C28" s="13" t="n"/>
-      <c r="D28" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="F28" s="10" t="n">
-        <v>0</v>
+      <c r="D28" s="9">
+        <f>SUMPRODUCT(('Upfront Carbon Reduction'!E6:E20&lt;&gt;"")*('Upfront Carbon Reduction'!G6:G20&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E28" s="9">
+        <f>COUNTA('Upfront Carbon Reduction'!E6:E20)</f>
+        <v/>
+      </c>
+      <c r="F28" s="10">
+        <f>IF(E28&gt;0,D28/E28,0)</f>
+        <v/>
       </c>
     </row>
     <row r="29" ht="22" customHeight="1">
@@ -1363,14 +1438,17 @@
         </is>
       </c>
       <c r="C29" s="13" t="n"/>
-      <c r="D29" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F29" s="10" t="n">
-        <v>0</v>
+      <c r="D29" s="9">
+        <f>SUMPRODUCT(('Upfront Carbon Compensation'!E6:E10&lt;&gt;"")*('Upfront Carbon Compensation'!G6:G10&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E29" s="9">
+        <f>COUNTA('Upfront Carbon Compensation'!E6:E10)</f>
+        <v/>
+      </c>
+      <c r="F29" s="10">
+        <f>IF(E29&gt;0,D29/E29,0)</f>
+        <v/>
       </c>
     </row>
     <row r="30" ht="22" customHeight="1">
@@ -1385,14 +1463,17 @@
         </is>
       </c>
       <c r="C30" s="13" t="n"/>
-      <c r="D30" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F30" s="10" t="n">
-        <v>0</v>
+      <c r="D30" s="9">
+        <f>SUMPRODUCT(('Refrigerant Systems Impacts'!E6:E13&lt;&gt;"")*('Refrigerant Systems Impacts'!G6:G13&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E30" s="9">
+        <f>COUNTA('Refrigerant Systems Impacts'!E6:E13)</f>
+        <v/>
+      </c>
+      <c r="F30" s="10">
+        <f>IF(E30&gt;0,D30/E30,0)</f>
+        <v/>
       </c>
     </row>
     <row r="31" ht="22" customHeight="1">
@@ -1407,14 +1488,17 @@
         </is>
       </c>
       <c r="C31" s="13" t="n"/>
-      <c r="D31" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F31" s="10" t="n">
-        <v>0</v>
+      <c r="D31" s="9">
+        <f>SUMPRODUCT(('Low-Emissions Transport'!E6:E11&lt;&gt;"")*('Low-Emissions Transport'!G6:G11&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E31" s="9">
+        <f>COUNTA('Low-Emissions Transport'!E6:E11)</f>
+        <v/>
+      </c>
+      <c r="F31" s="10">
+        <f>IF(E31&gt;0,D31/E31,0)</f>
+        <v/>
       </c>
     </row>
     <row r="32" ht="22" customHeight="1">
@@ -1429,14 +1513,17 @@
         </is>
       </c>
       <c r="C32" s="13" t="n"/>
-      <c r="D32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F32" s="10" t="n">
-        <v>0</v>
+      <c r="D32" s="9">
+        <f>SUMPRODUCT(('Design for Circularity'!E6:E14&lt;&gt;"")*('Design for Circularity'!G6:G14&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E32" s="9">
+        <f>COUNTA('Design for Circularity'!E6:E14)</f>
+        <v/>
+      </c>
+      <c r="F32" s="10">
+        <f>IF(E32&gt;0,D32/E32,0)</f>
+        <v/>
       </c>
     </row>
     <row r="33" ht="22" customHeight="1">
@@ -1451,14 +1538,17 @@
         </is>
       </c>
       <c r="C33" s="13" t="n"/>
-      <c r="D33" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F33" s="10" t="n">
-        <v>0</v>
+      <c r="D33" s="9">
+        <f>SUMPRODUCT(('Water Use'!E6:E16&lt;&gt;"")*('Water Use'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E33" s="9">
+        <f>COUNTA('Water Use'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F33" s="10">
+        <f>IF(E33&gt;0,D33/E33,0)</f>
+        <v/>
       </c>
     </row>
     <row r="34" ht="22" customHeight="1">
@@ -1473,14 +1563,17 @@
         </is>
       </c>
       <c r="C34" s="14" t="n"/>
-      <c r="D34" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F34" s="10" t="n">
-        <v>0</v>
+      <c r="D34" s="9">
+        <f>SUMPRODUCT(('Movement and Place'!E6:E13&lt;&gt;"")*('Movement and Place'!G6:G13&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E34" s="9">
+        <f>COUNTA('Movement and Place'!E6:E13)</f>
+        <v/>
+      </c>
+      <c r="F34" s="10">
+        <f>IF(E34&gt;0,D34/E34,0)</f>
+        <v/>
       </c>
     </row>
     <row r="35" ht="22" customHeight="1">
@@ -1495,14 +1588,17 @@
         </is>
       </c>
       <c r="C35" s="14" t="n"/>
-      <c r="D35" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F35" s="10" t="n">
-        <v>0</v>
+      <c r="D35" s="9">
+        <f>SUMPRODUCT(('Enjoyable Places'!E6:E12&lt;&gt;"")*('Enjoyable Places'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E35" s="9">
+        <f>COUNTA('Enjoyable Places'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F35" s="10">
+        <f>IF(E35&gt;0,D35/E35,0)</f>
+        <v/>
       </c>
     </row>
     <row r="36" ht="22" customHeight="1">
@@ -1517,14 +1613,17 @@
         </is>
       </c>
       <c r="C36" s="14" t="n"/>
-      <c r="D36" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F36" s="10" t="n">
-        <v>0</v>
+      <c r="D36" s="9">
+        <f>SUMPRODUCT(('Contribution to Place'!E6:E12&lt;&gt;"")*('Contribution to Place'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E36" s="9">
+        <f>COUNTA('Contribution to Place'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F36" s="10">
+        <f>IF(E36&gt;0,D36/E36,0)</f>
+        <v/>
       </c>
     </row>
     <row r="37" ht="22" customHeight="1">
@@ -1539,14 +1638,17 @@
         </is>
       </c>
       <c r="C37" s="14" t="n"/>
-      <c r="D37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F37" s="10" t="n">
-        <v>0</v>
+      <c r="D37" s="9">
+        <f>SUMPRODUCT(('Culture Heritage Identity'!E6:E10&lt;&gt;"")*('Culture Heritage Identity'!G6:G10&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E37" s="9">
+        <f>COUNTA('Culture Heritage Identity'!E6:E10)</f>
+        <v/>
+      </c>
+      <c r="F37" s="10">
+        <f>IF(E37&gt;0,D37/E37,0)</f>
+        <v/>
       </c>
     </row>
     <row r="38" ht="22" customHeight="1">
@@ -1561,14 +1663,17 @@
         </is>
       </c>
       <c r="C38" s="15" t="n"/>
-      <c r="D38" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F38" s="10" t="n">
-        <v>0</v>
+      <c r="D38" s="9">
+        <f>SUMPRODUCT(('Inclusive Construction'!E6:E15&lt;&gt;"")*('Inclusive Construction'!G6:G15&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E38" s="9">
+        <f>COUNTA('Inclusive Construction'!E6:E15)</f>
+        <v/>
+      </c>
+      <c r="F38" s="10">
+        <f>IF(E38&gt;0,D38/E38,0)</f>
+        <v/>
       </c>
     </row>
     <row r="39" ht="22" customHeight="1">
@@ -1583,14 +1688,17 @@
         </is>
       </c>
       <c r="C39" s="15" t="n"/>
-      <c r="D39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F39" s="10" t="n">
-        <v>0</v>
+      <c r="D39" s="9">
+        <f>SUMPRODUCT(('First Nations Inclusion'!E6:E12&lt;&gt;"")*('First Nations Inclusion'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E39" s="9">
+        <f>COUNTA('First Nations Inclusion'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F39" s="10">
+        <f>IF(E39&gt;0,D39/E39,0)</f>
+        <v/>
       </c>
     </row>
     <row r="40" ht="22" customHeight="1">
@@ -1605,14 +1713,17 @@
         </is>
       </c>
       <c r="C40" s="15" t="n"/>
-      <c r="D40" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F40" s="10" t="n">
-        <v>0</v>
+      <c r="D40" s="9">
+        <f>SUMPRODUCT(('Procurement Workforce Inclusion'!E6:E11&lt;&gt;"")*('Procurement Workforce Inclusion'!G6:G11&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E40" s="9">
+        <f>COUNTA('Procurement Workforce Inclusion'!E6:E11)</f>
+        <v/>
+      </c>
+      <c r="F40" s="10">
+        <f>IF(E40&gt;0,D40/E40,0)</f>
+        <v/>
       </c>
     </row>
     <row r="41" ht="22" customHeight="1">
@@ -1627,14 +1738,17 @@
         </is>
       </c>
       <c r="C41" s="15" t="n"/>
-      <c r="D41" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="9" t="n">
-        <v>8</v>
-      </c>
-      <c r="F41" s="10" t="n">
-        <v>0</v>
+      <c r="D41" s="9">
+        <f>SUMPRODUCT(('Design for Equity'!E6:E16&lt;&gt;"")*('Design for Equity'!G6:G16&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E41" s="9">
+        <f>COUNTA('Design for Equity'!E6:E16)</f>
+        <v/>
+      </c>
+      <c r="F41" s="10">
+        <f>IF(E41&gt;0,D41/E41,0)</f>
+        <v/>
       </c>
     </row>
     <row r="42" ht="22" customHeight="1">
@@ -1649,14 +1763,17 @@
         </is>
       </c>
       <c r="C42" s="16" t="n"/>
-      <c r="D42" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F42" s="10" t="n">
-        <v>0</v>
+      <c r="D42" s="9">
+        <f>SUMPRODUCT(('Impacts to Nature'!E6:E15&lt;&gt;"")*('Impacts to Nature'!G6:G15&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E42" s="9">
+        <f>COUNTA('Impacts to Nature'!E6:E15)</f>
+        <v/>
+      </c>
+      <c r="F42" s="10">
+        <f>IF(E42&gt;0,D42/E42,0)</f>
+        <v/>
       </c>
     </row>
     <row r="43" ht="22" customHeight="1">
@@ -1671,14 +1788,17 @@
         </is>
       </c>
       <c r="C43" s="16" t="n"/>
-      <c r="D43" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F43" s="10" t="n">
-        <v>0</v>
+      <c r="D43" s="9">
+        <f>SUMPRODUCT(('Biodiversity Enhancement'!E6:E12&lt;&gt;"")*('Biodiversity Enhancement'!G6:G12&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E43" s="9">
+        <f>COUNTA('Biodiversity Enhancement'!E6:E12)</f>
+        <v/>
+      </c>
+      <c r="F43" s="10">
+        <f>IF(E43&gt;0,D43/E43,0)</f>
+        <v/>
       </c>
     </row>
     <row r="44" ht="22" customHeight="1">
@@ -1693,14 +1813,17 @@
         </is>
       </c>
       <c r="C44" s="16" t="n"/>
-      <c r="D44" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F44" s="10" t="n">
-        <v>0</v>
+      <c r="D44" s="9">
+        <f>SUMPRODUCT(('Nature Connectivity'!E6:E13&lt;&gt;"")*('Nature Connectivity'!G6:G13&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E44" s="9">
+        <f>COUNTA('Nature Connectivity'!E6:E13)</f>
+        <v/>
+      </c>
+      <c r="F44" s="10">
+        <f>IF(E44&gt;0,D44/E44,0)</f>
+        <v/>
       </c>
     </row>
     <row r="45" ht="22" customHeight="1">
@@ -1715,14 +1838,17 @@
         </is>
       </c>
       <c r="C45" s="16" t="n"/>
-      <c r="D45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F45" s="10" t="n">
-        <v>0</v>
+      <c r="D45" s="9">
+        <f>SUMPRODUCT(('Nature Stewardship'!E6:E11&lt;&gt;"")*('Nature Stewardship'!G6:G11&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E45" s="9">
+        <f>COUNTA('Nature Stewardship'!E6:E11)</f>
+        <v/>
+      </c>
+      <c r="F45" s="10">
+        <f>IF(E45&gt;0,D45/E45,0)</f>
+        <v/>
       </c>
     </row>
     <row r="46" ht="22" customHeight="1">
@@ -1737,14 +1863,17 @@
         </is>
       </c>
       <c r="C46" s="16" t="n"/>
-      <c r="D46" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="F46" s="10" t="n">
-        <v>0</v>
+      <c r="D46" s="9">
+        <f>SUMPRODUCT(('Waterway Protection'!E6:E15&lt;&gt;"")*('Waterway Protection'!G6:G15&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E46" s="9">
+        <f>COUNTA('Waterway Protection'!E6:E15)</f>
+        <v/>
+      </c>
+      <c r="F46" s="10">
+        <f>IF(E46&gt;0,D46/E46,0)</f>
+        <v/>
       </c>
     </row>
     <row r="47" ht="22" customHeight="1">
@@ -1759,14 +1888,17 @@
         </is>
       </c>
       <c r="C47" s="17" t="n"/>
-      <c r="D47" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="F47" s="10" t="n">
-        <v>0</v>
+      <c r="D47" s="9">
+        <f>SUMPRODUCT(('Market Transformation'!E6:E11&lt;&gt;"")*('Market Transformation'!G6:G11&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E47" s="9">
+        <f>COUNTA('Market Transformation'!E6:E11)</f>
+        <v/>
+      </c>
+      <c r="F47" s="10">
+        <f>IF(E47&gt;0,D47/E47,0)</f>
+        <v/>
       </c>
     </row>
     <row r="48" ht="22" customHeight="1">
@@ -1781,14 +1913,17 @@
         </is>
       </c>
       <c r="C48" s="17" t="n"/>
-      <c r="D48" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F48" s="10" t="n">
-        <v>0</v>
+      <c r="D48" s="9">
+        <f>SUMPRODUCT(('Leadership Challenges'!E6:E9&lt;&gt;"")*('Leadership Challenges'!G6:G9&lt;&gt;""))</f>
+        <v/>
+      </c>
+      <c r="E48" s="9">
+        <f>COUNTA('Leadership Challenges'!E6:E9)</f>
+        <v/>
+      </c>
+      <c r="F48" s="10">
+        <f>IF(E48&gt;0,D48/E48,0)</f>
+        <v/>
       </c>
     </row>
     <row r="50">
@@ -1847,14 +1982,14 @@
     <row r="55">
       <c r="A55" s="21" t="inlineStr">
         <is>
-          <t>• Y/N questions use dropdown validation - dependent questions show/hide automatically</t>
+          <t>• Y/N questions use dropdown validation</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="21" t="inlineStr">
         <is>
-          <t>• Use the action buttons above: Review highlights gaps, Search finds questions across credits</t>
+          <t>• Progress updates automatically via formulas (Answered / Total / %)</t>
         </is>
       </c>
     </row>
@@ -1868,31 +2003,31 @@
     <row r="58">
       <c r="A58" s="21" t="inlineStr">
         <is>
-          <t>• To mark a credit as N/A: go to the credit sheet and run the N/A toggle (macros menu)</t>
+          <t>• Sheets are protected — only the Response column is editable (password: greenstar)</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="21" t="inlineStr">
-        <is>
-          <t>• Progress updates automatically when you change responses</t>
-        </is>
-      </c>
+      <c r="A59" s="21" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" s="21" t="inlineStr"/>
+      <c r="A60" s="21" t="inlineStr">
+        <is>
+          <t>OPTIONAL VBA MACROS (for advanced features):</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="21" t="inlineStr">
         <is>
-          <t>KEYBOARD SHORTCUTS (via macros):</t>
+          <t>• Save as .xlsm, then import GreenStarMacros.bas via Developer &gt; Visual Basic &gt; File &gt; Import</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="21" t="inlineStr">
         <is>
-          <t>• Ctrl+Shift+D = Dashboard  |  Ctrl+Shift+S = Search  |  Ctrl+Shift+R = Review</t>
+          <t>• Adds: conditional row visibility, search, review mode, dark mode, version history</t>
         </is>
       </c>
     </row>

</xml_diff>